<commit_message>
se avanzó en la question, fachada, enum y query de consulta saldos tarjetas de credito
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Canales\AW1059001_APPSucursalVirtualPersonas_Test\APP_PERSONAS\src\test\resources\datadriven\consultas\saldos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2079D3-7F20-4CED-BABA-A4F4C8496D19}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7695" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -103,15 +109,6 @@
     <t>406-101390-08;406101390-09;406-701390-12;406-701390-13</t>
   </si>
   <si>
-    <t>creadoosp11</t>
-  </si>
-  <si>
-    <t>Personal American Express;Personal American Express;Personal American Express;Personal Visa;Personal Visa;Personal Visa;Personal Mastercard;Personal Mastercard;Personal Mastercard;Personal Mastercard</t>
-  </si>
-  <si>
-    <t>*0350;*9056;*6269;*7757;*1597;*0606;*6095;*7287;*4452;*2390</t>
-  </si>
-  <si>
     <t>usercdt66</t>
   </si>
   <si>
@@ -173,19 +170,28 @@
   </si>
   <si>
     <t>Consultas</t>
+  </si>
+  <si>
+    <t>58156998</t>
+  </si>
+  <si>
+    <t>automata98</t>
+  </si>
+  <si>
+    <t>0260</t>
+  </si>
+  <si>
+    <t>Personal American Express;Personal Visa;Personal Mastercard</t>
+  </si>
+  <si>
+    <t>*4379;*2391;*0299</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -209,158 +215,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -385,194 +247,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -595,254 +271,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -854,65 +288,22 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="Normal 2" xfId="32"/>
-    <cellStyle name="20% - Accent5" xfId="33" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="34" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="35" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="36" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="38" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="39" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="40" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="41" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="42" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="43" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="44" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="45" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="46" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="47" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="48" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="49" builtinId="52"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1170,26 +561,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.08203125" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.08203125" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.58203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1280,7 +671,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1294,7 +685,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1309,34 +700,41 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.08203125" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.08203125" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="52.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="56.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1388,13 +786,13 @@
         <v>14</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>17</v>
@@ -1405,13 +803,13 @@
       <c r="G2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="I2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" t="s">
         <v>22</v>
       </c>
       <c r="K2" s="12" t="s">
@@ -1421,13 +819,13 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1441,7 +839,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1456,34 +854,39 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G4 H3:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.08203125" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.08203125" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.58203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1541,7 +944,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>17</v>
@@ -1568,13 +971,13 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1588,7 +991,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1603,34 +1006,39 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.08203125" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.08203125" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.58203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1717,7 +1125,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1731,7 +1139,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1746,34 +1154,39 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.08203125" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.08203125" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.58203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1858,13 +1271,13 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1878,7 +1291,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1893,34 +1306,39 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.08203125" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.08203125" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.58203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2007,7 +1425,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -2021,7 +1439,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -2036,46 +1454,51 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
-    <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="1" max="1" width="10.58203125" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.08203125" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
         <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2083,54 +1506,54 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>44</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
-      <c r="B4" t="s">
+    <row r="6" spans="1:4">
+      <c r="B6" t="s">
         <v>46</v>
       </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2">
-      <c r="B5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2">
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2">
-      <c r="B7" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se realiza el desarrollo del componente COMFFLGWWW para la transaccion consulta saldos creditos 0345
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosmarioloperamurillo/Documents/ProyectosIntellij/AW1059001_NuevaAPPSucursalVirtualPersonas_Test/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1612D781-751C-F042-93DC-ED06B8F94834}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7695" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -112,15 +118,6 @@
     <t>*0350;*9056;*6269;*7757;*1597;*0606;*6095;*7287;*4452;*2390</t>
   </si>
   <si>
-    <t>usercdt66</t>
-  </si>
-  <si>
-    <t>Prestamo Personal Ta;Prestamo Personal Ta</t>
-  </si>
-  <si>
-    <t>29281005510;29281023970</t>
-  </si>
-  <si>
     <t>MasterCard</t>
   </si>
   <si>
@@ -173,19 +170,25 @@
   </si>
   <si>
     <t>Consultas</t>
+  </si>
+  <si>
+    <t>invictus12</t>
+  </si>
+  <si>
+    <t>0345</t>
+  </si>
+  <si>
+    <t>Prestamo Personal Ta</t>
+  </si>
+  <si>
+    <t>292810023955</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -209,158 +212,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -385,194 +244,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -595,254 +268,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -854,65 +285,21 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="Normal 2" xfId="32"/>
-    <cellStyle name="20% - Accent5" xfId="33" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="34" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="35" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="36" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="38" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="39" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="40" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="41" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="42" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="43" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="44" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="45" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="46" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="47" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="48" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="49" builtinId="52"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1170,26 +557,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1280,7 +667,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1294,7 +681,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1309,34 +696,39 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1427,7 +819,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1441,7 +833,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1456,34 +848,39 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1534,14 +931,14 @@
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>15</v>
+      <c r="B2" s="11">
+        <v>22419862</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>17</v>
@@ -1556,7 +953,7 @@
         <v>20</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>22</v>
@@ -1568,13 +965,13 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1588,7 +985,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1603,34 +1000,39 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:H4 J2:J4 I3:I4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1717,7 +1119,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1731,7 +1133,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1746,34 +1148,39 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1858,13 +1265,13 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1878,7 +1285,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1893,34 +1300,39 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2007,7 +1419,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -2021,7 +1433,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -2036,46 +1448,51 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
-    <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
         <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2083,54 +1500,53 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>44</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
-      <c r="B4" t="s">
+    <row r="6" spans="1:4">
+      <c r="B6" t="s">
         <v>46</v>
       </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2">
-      <c r="B5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2">
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2">
-      <c r="B7" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se realiza la estabilizacion de los componentes log canal y cxref - cname y lmbal para la transaccion consulta de creditos 0345
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosmarioloperamurillo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosmarioloperamurillo/Documents/ProyectosIntellij/AW1059001_NuevaAPPSucursalVirtualPersonas_Test/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B9393E-15B9-F84F-B7BA-9AF287DF9387}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2A975F-C410-0141-9DEE-8E5C3548B3AE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20500" windowHeight="7700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -193,7 +193,7 @@
     <t>Prestamo Personal Ta</t>
   </si>
   <si>
-    <t>292810023955</t>
+    <t>29281023955</t>
   </si>
 </sst>
 </file>
@@ -891,7 +891,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1034,7 +1034,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{688B3D4C-F3F9-0248-B3EA-00272EB901E0}">
           <x14:formula1>
-            <xm:f>[ConsultaSaldosConsolidados.xlsx]Listas!#REF!</xm:f>
+            <xm:f>Listas!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>G2:H2 J2</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
se realizaron cambios en las clases con el fin de buscar estabilizar la transaccion
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Canales\AW1059001_APPSucursalVirtualPersonas_Test\APP_PERSONAS\src\test\resources\datadriven\consultas\saldos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel.rios.cano/Documents/AW1059001_APPSucursalVirtualPersonas_Test/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2079D3-7F20-4CED-BABA-A4F4C8496D19}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4794B7-CECA-7440-A56E-D922E4C43504}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -573,14 +573,14 @@
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.08203125" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="6" width="14.33203125" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="22.08203125" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="14.58203125" customWidth="1"/>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -721,19 +721,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.08203125" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="6" width="14.33203125" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="22.08203125" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
     <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="52.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="56.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -879,14 +879,14 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.08203125" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="6" width="14.33203125" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="22.08203125" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="14.58203125" customWidth="1"/>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1031,14 +1031,14 @@
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.08203125" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="6" width="14.33203125" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="22.08203125" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="14.58203125" customWidth="1"/>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1179,14 +1179,14 @@
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.08203125" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="6" width="14.33203125" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="22.08203125" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="14.58203125" customWidth="1"/>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1331,14 +1331,14 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.08203125" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="6" width="14.33203125" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="22.08203125" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="14.58203125" customWidth="1"/>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1479,11 +1479,11 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.58203125" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.08203125" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
se desarrolla y estabilizan las transacciones consulta de saldos de creditos y depositos con la nueva estrategia para el mapeo de los objetos
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosmarioloperamurillo/Documents/ProyectosIntellij/AW1059001_NuevaAPPSucursalVirtualPersonas_Test/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2A975F-C410-0141-9DEE-8E5C3548B3AE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E0030A-CD50-2546-8374-21CF52F69664}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -178,34 +178,41 @@
     <t>22452521</t>
   </si>
   <si>
+    <t>invictus12</t>
+  </si>
+  <si>
+    <t>0345</t>
+  </si>
+  <si>
+    <t>Prestamo Personal Ta</t>
+  </si>
+  <si>
+    <t>29281023955</t>
+  </si>
+  <si>
     <t>406-125210-00;406-125210-01;406-125210-02;406-725210-11;406-725210-12;406-725210-13;406-725210-14</t>
   </si>
   <si>
-    <t>Corriente;Corriente;Corriente;Ahorros;Ahorros;Ahorros;Ahorros</t>
-  </si>
-  <si>
-    <t>invictus12</t>
-  </si>
-  <si>
-    <t>0345</t>
-  </si>
-  <si>
-    <t>Prestamo Personal Ta</t>
-  </si>
-  <si>
-    <t>29281023955</t>
+    <t>Corriente;Corriente;Adelanto;Ahorros;Ahorros;Ahorros;Ahorros</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -283,27 +290,29 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -681,11 +690,11 @@
       <c r="L2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>50</v>
+      <c r="M2" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -890,7 +899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -959,7 +968,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>17</v>
@@ -974,7 +983,7 @@
         <v>20</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>22</v>
@@ -986,10 +995,10 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:14">

</xml_diff>

<commit_message>
se estabiliza saldos consolidados de los productos
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7695" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7695" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -130,7 +130,7 @@
     <t>MasterCard</t>
   </si>
   <si>
-    <t>5306950634968354</t>
+    <t>*8354</t>
   </si>
   <si>
     <t>Orientacion</t>
@@ -216,6 +216,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -223,16 +230,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -258,6 +266,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -274,26 +305,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -313,6 +328,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -322,49 +359,12 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -393,19 +393,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -417,13 +555,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -435,102 +567,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -538,42 +574,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -602,11 +602,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -615,6 +621,17 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -638,23 +655,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -688,163 +699,152 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -857,9 +857,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
@@ -1235,10 +1235,10 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1267,7 +1267,7 @@
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -1295,7 +1295,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="10"/>
+      <c r="I3" s="9"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
@@ -1331,7 +1331,7 @@
   <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
@@ -1382,10 +1382,10 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1414,7 +1414,7 @@
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -1442,7 +1442,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="10"/>
+      <c r="I3" s="9"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
@@ -1529,10 +1529,10 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1561,7 +1561,7 @@
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -1589,7 +1589,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="10"/>
+      <c r="I3" s="9"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
@@ -1676,10 +1676,10 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1708,7 +1708,7 @@
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -1736,7 +1736,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="10"/>
+      <c r="I3" s="9"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
@@ -1773,7 +1773,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
@@ -1823,10 +1823,10 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1855,7 +1855,7 @@
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -1883,7 +1883,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="10"/>
+      <c r="I3" s="9"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
@@ -1917,10 +1917,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
@@ -1933,7 +1933,7 @@
     <col min="12" max="12" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1970,14 +1970,8 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
@@ -2002,7 +1996,7 @@
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -2014,8 +2008,6 @@
       <c r="L2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="5"/>
@@ -2026,7 +2018,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="10"/>
+      <c r="I3" s="9"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>

</xml_diff>

<commit_message>
se realiza pull a la rama develop para actualizar proyecto APP
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel.rios.cano/Documents/AW1059001_APPSucursalVirtualPersonas_Test/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4794B7-CECA-7440-A56E-D922E4C43504}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8925786-9C1F-8743-934F-8FD2463756AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -181,10 +181,10 @@
     <t>0260</t>
   </si>
   <si>
-    <t>Personal American Express;Personal Visa;Personal Mastercard</t>
-  </si>
-  <si>
     <t>*4379;*2391;*0299</t>
+  </si>
+  <si>
+    <t>CREDIT_CARD;CREDIT_CARD;CREDIT_CARD</t>
   </si>
 </sst>
 </file>
@@ -722,7 +722,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -819,10 +819,10 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:14">

</xml_diff>

<commit_message>
se ha completado la transaccion de consulta de saldos tarjetas de credito back e integracion
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel.rios.cano/Documents/AW1059001_APPSucursalVirtualPersonas_Test/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8925786-9C1F-8743-934F-8FD2463756AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C46F676-8E7A-F240-9FB5-CDCCBB88DC6E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -184,14 +184,14 @@
     <t>*4379;*2391;*0299</t>
   </si>
   <si>
-    <t>CREDIT_CARD;CREDIT_CARD;CREDIT_CARD</t>
+    <t>Personal American Express;Personal Visa;Personal Mastercard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -220,6 +220,12 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -276,7 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -291,6 +297,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,7 +729,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -818,7 +825,7 @@
       <c r="L2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="14" t="s">
         <v>52</v>
       </c>
       <c r="N2" s="3" t="s">

</xml_diff>

<commit_message>
Estabilizacion consulta de saldos tarjeta de credito
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/bancolombia-app-personas-osp-tests-bdd-screen-play/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7695" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -15,12 +20,18 @@
     <sheet name="Crediagil" sheetId="7" r:id="rId6"/>
     <sheet name="Listas" sheetId="2" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -106,21 +117,12 @@
     <t>1037655531</t>
   </si>
   <si>
-    <t>creadoosp11</t>
-  </si>
-  <si>
     <t>0369</t>
   </si>
   <si>
     <t>NO ERROR</t>
   </si>
   <si>
-    <t>Personal American Express;Personal American Express;Personal American Express;Personal Visa;Personal Visa;Personal Visa;Personal Mastercard;Personal Mastercard;Personal Mastercard;Personal Mastercard</t>
-  </si>
-  <si>
-    <t>*0350;*9056;*6269;*7757;*1597;*0606;*6095;*7287;*4452;*2390</t>
-  </si>
-  <si>
     <t>invictus12</t>
   </si>
   <si>
@@ -203,24 +205,30 @@
   </si>
   <si>
     <t>Consultas</t>
+  </si>
+  <si>
+    <t>pruebauser01</t>
+  </si>
+  <si>
+    <t>6789</t>
+  </si>
+  <si>
+    <t>Personal American Express;Personal American Express;Personal Visa</t>
+  </si>
+  <si>
+    <t>*8410;*3490;*6177</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -245,159 +253,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,194 +279,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -632,254 +303,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -897,62 +326,15 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="Normal 2" xfId="32"/>
-    <cellStyle name="20% - Accent5" xfId="33" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="34" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="35" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="36" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="38" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="39" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="40" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="41" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="42" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="43" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="44" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="45" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="46" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="47" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="48" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="49" builtinId="52"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1214,33 +596,33 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.125" style="11" customWidth="1"/>
-    <col min="2" max="6" width="14.375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" style="11" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" style="11" customWidth="1"/>
     <col min="7" max="7" width="13.5" style="11" customWidth="1"/>
-    <col min="8" max="9" width="14.375" style="11" customWidth="1"/>
-    <col min="10" max="10" width="20.375" style="11" customWidth="1"/>
-    <col min="11" max="11" width="14.375" style="11" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="11" customWidth="1"/>
+    <col min="8" max="9" width="14.33203125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="11" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" style="11" customWidth="1"/>
     <col min="13" max="13" width="30" style="11" customWidth="1"/>
     <col min="14" max="14" width="91.5" style="11" customWidth="1"/>
     <col min="15" max="16384" width="11" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1284,7 +666,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>14</v>
       </c>
@@ -1328,7 +710,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="6"/>
@@ -1342,7 +724,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4" s="6"/>
       <c r="C4" s="13"/>
@@ -1357,37 +739,42 @@
       <c r="L4" s="13"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1431,7 +818,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>14</v>
       </c>
@@ -1442,10 +829,10 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>18</v>
@@ -1457,10 +844,10 @@
         <v>20</v>
       </c>
       <c r="I2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>23</v>
@@ -1469,13 +856,13 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1489,7 +876,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1504,37 +891,32 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
-  <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1578,7 +960,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>14</v>
       </c>
@@ -1589,7 +971,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>17</v>
@@ -1604,10 +986,10 @@
         <v>20</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K2" s="17" t="s">
         <v>23</v>
@@ -1616,13 +998,13 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="N2" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1636,7 +1018,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1651,43 +1033,32 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H2;J2">
-      <formula1>Listas!#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="13.5" style="11" customWidth="1"/>
-    <col min="8" max="9" width="14.375" style="11" customWidth="1"/>
-    <col min="10" max="10" width="20.375" style="11" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
-    <col min="13" max="13" width="23.375" customWidth="1"/>
-    <col min="14" max="14" width="27.75" customWidth="1"/>
+    <col min="8" max="9" width="14.33203125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="13" max="13" width="23.33203125" customWidth="1"/>
+    <col min="14" max="14" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1731,7 +1102,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>14</v>
       </c>
@@ -1757,7 +1128,7 @@
         <v>20</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J2" s="18" t="s">
         <v>22</v>
@@ -1769,13 +1140,13 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1789,7 +1160,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1804,40 +1175,45 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="13.5" style="11" customWidth="1"/>
-    <col min="8" max="9" width="14.375" style="11" customWidth="1"/>
-    <col min="10" max="10" width="20.375" style="11" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
-    <col min="13" max="13" width="10.375" customWidth="1"/>
-    <col min="14" max="14" width="13.625" customWidth="1"/>
+    <col min="8" max="9" width="14.33203125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1881,12 +1257,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>14</v>
@@ -1907,7 +1283,7 @@
         <v>20</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J2" s="18" t="s">
         <v>22</v>
@@ -1919,13 +1295,13 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="N2" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1939,7 +1315,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1954,37 +1330,42 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2028,7 +1409,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>14</v>
       </c>
@@ -2039,7 +1420,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>17</v>
@@ -2054,10 +1435,10 @@
         <v>20</v>
       </c>
       <c r="I2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>23</v>
@@ -2068,7 +1449,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -2082,7 +1463,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -2097,101 +1478,105 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
-    <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>49</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>50</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
         <v>52</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>53</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>54</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
-      <c r="B4" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>56</v>
       </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2">
-      <c r="B5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2">
-      <c r="B6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2">
-      <c r="B7" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactorización archivos .feature, se elimina la linea de cierre de sesión
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOSP\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\consultas\saldos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C9EB50-CFB1-499C-98AA-7F5B3842FBF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7695" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -202,14 +208,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -239,159 +239,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -416,194 +265,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -626,254 +289,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -891,66 +312,24 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="Normal 2" xfId="32"/>
-    <cellStyle name="20% - Accent5" xfId="33" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="34" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="35" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="36" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="38" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="39" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="40" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="41" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="42" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="43" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="44" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="45" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="46" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="47" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="48" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="49" builtinId="52"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1208,27 +587,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="11.1666666666667" style="11" customWidth="1"/>
-    <col min="2" max="6" width="14.3333333333333" style="11" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" style="11" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" style="11" customWidth="1"/>
     <col min="7" max="7" width="13.5" style="11" customWidth="1"/>
-    <col min="8" max="9" width="14.3333333333333" style="11" customWidth="1"/>
-    <col min="10" max="10" width="20.3333333333333" style="11" customWidth="1"/>
-    <col min="11" max="11" width="14.3333333333333" style="11" customWidth="1"/>
-    <col min="12" max="12" width="14.6666666666667" style="11" customWidth="1"/>
+    <col min="8" max="9" width="14.33203125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="11" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" style="11" customWidth="1"/>
     <col min="13" max="13" width="30" style="11" customWidth="1"/>
     <col min="14" max="14" width="91.5" style="11" customWidth="1"/>
     <col min="15" max="16384" width="11" style="11"/>
@@ -1322,7 +701,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="6"/>
@@ -1336,7 +715,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="13"/>
       <c r="B4" s="6"/>
       <c r="C4" s="13"/>
@@ -1351,34 +730,39 @@
       <c r="L4" s="13"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="11.1666666666667" customWidth="1"/>
-    <col min="2" max="6" width="14.3333333333333" customWidth="1"/>
-    <col min="9" max="9" width="18.3333333333333" customWidth="1"/>
-    <col min="10" max="10" width="22.1666666666667" customWidth="1"/>
-    <col min="11" max="11" width="14.3333333333333" customWidth="1"/>
-    <col min="12" max="12" width="14.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1469,7 +853,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1483,7 +867,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1498,27 +882,32 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
@@ -1608,7 +997,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1622,7 +1011,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1638,30 +1027,28 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="11.1666666666667" customWidth="1"/>
-    <col min="2" max="6" width="14.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="13.5" style="11" customWidth="1"/>
-    <col min="8" max="9" width="14.3333333333333" style="11" customWidth="1"/>
-    <col min="10" max="10" width="20.3333333333333" style="11" customWidth="1"/>
-    <col min="11" max="11" width="14.3333333333333" customWidth="1"/>
-    <col min="12" max="12" width="14.6666666666667" customWidth="1"/>
-    <col min="13" max="13" width="23.3333333333333" customWidth="1"/>
-    <col min="14" max="14" width="27.6666666666667" customWidth="1"/>
+    <col min="8" max="9" width="14.33203125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="13" max="13" width="23.33203125" customWidth="1"/>
+    <col min="14" max="14" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1752,7 +1139,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1766,7 +1153,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1781,37 +1168,42 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="11.1666666666667" customWidth="1"/>
-    <col min="2" max="6" width="14.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="13.5" style="11" customWidth="1"/>
-    <col min="8" max="9" width="14.3333333333333" style="11" customWidth="1"/>
-    <col min="10" max="10" width="20.3333333333333" style="11" customWidth="1"/>
-    <col min="11" max="11" width="14.3333333333333" customWidth="1"/>
-    <col min="12" max="12" width="14.6666666666667" customWidth="1"/>
-    <col min="13" max="13" width="10.3333333333333" customWidth="1"/>
-    <col min="14" max="14" width="13.6666666666667" customWidth="1"/>
+    <col min="8" max="9" width="14.33203125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1902,7 +1294,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1916,7 +1308,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1931,34 +1323,39 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="11.1666666666667" customWidth="1"/>
-    <col min="2" max="6" width="14.3333333333333" customWidth="1"/>
-    <col min="9" max="9" width="18.3333333333333" customWidth="1"/>
-    <col min="10" max="10" width="22.1666666666667" customWidth="1"/>
-    <col min="11" max="11" width="14.3333333333333" customWidth="1"/>
-    <col min="12" max="12" width="14.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1998,12 +1395,8 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>13</v>
-      </c>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="19" t="s">
@@ -2042,10 +1435,10 @@
       <c r="L2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -2059,7 +1452,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -2074,32 +1467,37 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="10.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="14.8333333333333" customWidth="1"/>
-    <col min="3" max="3" width="12.1666666666667" customWidth="1"/>
-    <col min="4" max="4" width="17.8333333333333" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2144,7 +1542,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>54</v>
       </c>
@@ -2152,23 +1550,22 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="1:4">
       <c r="B5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="1:4">
       <c r="B6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
consulta productos depositos vista carrusel
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOSP\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\consultas\saldos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\OSP_NEW\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\consultas\saldos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C9EB50-CFB1-499C-98AA-7F5B3842FBF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -21,12 +20,12 @@
     <sheet name="Crediagil" sheetId="7" r:id="rId6"/>
     <sheet name="Listas" sheetId="2" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -203,12 +202,21 @@
   </si>
   <si>
     <t>Consultas</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>numeroProductos</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="12"/>
@@ -294,7 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -311,7 +319,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -320,7 +327,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -592,28 +599,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" style="11" customWidth="1"/>
-    <col min="2" max="6" width="14.33203125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="11.125" style="11" customWidth="1"/>
+    <col min="2" max="6" width="14.375" style="11" customWidth="1"/>
     <col min="7" max="7" width="13.5" style="11" customWidth="1"/>
-    <col min="8" max="9" width="14.33203125" style="11" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" style="11" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" style="11" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" style="11" customWidth="1"/>
+    <col min="8" max="9" width="14.375" style="11" customWidth="1"/>
+    <col min="10" max="10" width="20.375" style="11" customWidth="1"/>
+    <col min="11" max="11" width="14.375" style="11" customWidth="1"/>
+    <col min="12" max="12" width="14.625" style="11" customWidth="1"/>
     <col min="13" max="13" width="30" style="11" customWidth="1"/>
-    <col min="14" max="14" width="91.5" style="11" customWidth="1"/>
-    <col min="15" max="16384" width="11" style="11"/>
+    <col min="14" max="14" width="104.625" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="11" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -656,66 +664,99 @@
       <c r="N1" s="14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="17" t="s">
+      <c r="O1" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="17" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="13"/>
       <c r="B4" s="6"/>
       <c r="C4" s="13"/>
@@ -735,7 +776,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -748,21 +789,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="6" width="14.33203125" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="22.1640625" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.125" customWidth="1"/>
+    <col min="2" max="6" width="14.375" customWidth="1"/>
+    <col min="9" max="9" width="18.375" customWidth="1"/>
+    <col min="10" max="10" width="22.125" customWidth="1"/>
+    <col min="11" max="11" width="14.375" customWidth="1"/>
+    <col min="12" max="12" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -810,22 +851,22 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -840,10 +881,10 @@
       <c r="J2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="17" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
@@ -887,7 +928,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -900,14 +941,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
@@ -954,22 +995,22 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="3">
         <v>22419862</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="12" t="s">
@@ -984,16 +1025,16 @@
       <c r="J2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="16" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="16" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1031,24 +1072,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.125" customWidth="1"/>
+    <col min="2" max="6" width="14.375" customWidth="1"/>
     <col min="7" max="7" width="13.5" style="11" customWidth="1"/>
-    <col min="8" max="9" width="14.33203125" style="11" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" style="11" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
-    <col min="13" max="13" width="23.33203125" customWidth="1"/>
-    <col min="14" max="14" width="27.6640625" customWidth="1"/>
+    <col min="8" max="9" width="14.375" style="11" customWidth="1"/>
+    <col min="10" max="10" width="20.375" style="11" customWidth="1"/>
+    <col min="11" max="11" width="14.375" customWidth="1"/>
+    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="13" max="13" width="23.375" customWidth="1"/>
+    <col min="14" max="14" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1096,40 +1137,40 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="17" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
@@ -1173,7 +1214,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -1186,24 +1227,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.125" customWidth="1"/>
+    <col min="2" max="6" width="14.375" customWidth="1"/>
     <col min="7" max="7" width="13.5" style="11" customWidth="1"/>
-    <col min="8" max="9" width="14.33203125" style="11" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" style="11" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" customWidth="1"/>
+    <col min="8" max="9" width="14.375" style="11" customWidth="1"/>
+    <col min="10" max="10" width="20.375" style="11" customWidth="1"/>
+    <col min="11" max="11" width="14.375" customWidth="1"/>
+    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="13" max="13" width="10.375" customWidth="1"/>
+    <col min="14" max="14" width="13.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1251,46 +1292,46 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="17" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="19" t="s">
+      <c r="N2" s="18" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1328,7 +1369,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -1341,21 +1382,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:N2"/>
+    <sheetView topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="6" width="14.33203125" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="22.1640625" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.125" customWidth="1"/>
+    <col min="2" max="6" width="14.375" customWidth="1"/>
+    <col min="9" max="9" width="18.375" customWidth="1"/>
+    <col min="10" max="10" width="22.125" customWidth="1"/>
+    <col min="11" max="11" width="14.375" customWidth="1"/>
+    <col min="12" max="12" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1395,26 +1436,26 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1429,14 +1470,14 @@
       <c r="J2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="5"/>
@@ -1472,7 +1513,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -1485,19 +1526,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1"/>
+    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="4" max="4" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
avances consulta productos tarjeta credito vista carrusel
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>1037655531</t>
-  </si>
-  <si>
-    <t>6789</t>
   </si>
   <si>
     <t>0369</t>
@@ -602,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
@@ -665,7 +662,7 @@
         <v>13</v>
       </c>
       <c r="O1" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -715,7 +712,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>15</v>
@@ -753,7 +750,7 @@
       <c r="M3" s="15"/>
       <c r="N3" s="15"/>
       <c r="O3" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -792,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -864,7 +861,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>18</v>
@@ -876,10 +873,10 @@
         <v>20</v>
       </c>
       <c r="I2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="K2" s="17" t="s">
         <v>23</v>
@@ -888,10 +885,10 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1020,10 +1017,10 @@
         <v>20</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K2" s="16" t="s">
         <v>23</v>
@@ -1032,10 +1029,10 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="16" t="s">
         <v>34</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1162,7 +1159,7 @@
         <v>20</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>22</v>
@@ -1174,10 +1171,10 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1296,7 +1293,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>14</v>
@@ -1317,7 +1314,7 @@
         <v>20</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>22</v>
@@ -1329,10 +1326,10 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="18" t="s">
         <v>41</v>
-      </c>
-      <c r="N2" s="18" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1465,10 +1462,10 @@
         <v>20</v>
       </c>
       <c r="I2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="K2" s="17" t="s">
         <v>23</v>
@@ -1543,16 +1540,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>45</v>
-      </c>
-      <c r="D1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1560,50 +1557,50 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
         <v>50</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>51</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
         <v>54</v>
-      </c>
-      <c r="D4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
avances saldos consolidados vista carrusel eprepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -207,10 +207,10 @@
     <t>numeroProductos</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>6</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -603,7 +603,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O3"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -753,7 +753,7 @@
       <c r="M3" s="15"/>
       <c r="N3" s="15"/>
       <c r="O3" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -940,7 +940,7 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -977,15 +977,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="14" max="14" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1028,8 +1032,11 @@
       <c r="N1" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="18" t="s">
         <v>14</v>
       </c>
@@ -1072,22 +1079,52 @@
       <c r="N2" s="16" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="3">
+        <v>22419862</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="3"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1263,10 +1300,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1280,9 +1317,10 @@
     <col min="12" max="12" width="14.625" customWidth="1"/>
     <col min="13" max="13" width="10.375" customWidth="1"/>
     <col min="14" max="14" width="13.625" customWidth="1"/>
+    <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1325,8 +1363,11 @@
       <c r="N1" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="18" t="s">
         <v>14</v>
       </c>
@@ -1369,22 +1410,52 @@
       <c r="N2" s="18" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="3"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>

</xml_diff>

<commit_message>
fin automatizacion consulta saldos todos los productos vista carrusel
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/saldos/ConsultaSaldosConsolidados.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="4"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -217,7 +217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -247,6 +247,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -274,7 +281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -297,12 +304,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -313,7 +333,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -322,8 +341,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,23 +626,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="11.125" style="11" customWidth="1"/>
-    <col min="2" max="6" width="14.375" style="11" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="11" customWidth="1"/>
-    <col min="8" max="9" width="14.375" style="11" customWidth="1"/>
-    <col min="10" max="10" width="20.375" style="11" customWidth="1"/>
-    <col min="11" max="11" width="14.375" style="11" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="11" customWidth="1"/>
-    <col min="13" max="13" width="30" style="11" customWidth="1"/>
-    <col min="14" max="14" width="104.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="11" style="11"/>
+    <col min="1" max="1" width="11.125" style="10" customWidth="1"/>
+    <col min="2" max="6" width="14.375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="10" customWidth="1"/>
+    <col min="8" max="9" width="14.375" style="10" customWidth="1"/>
+    <col min="10" max="10" width="20.375" style="10" customWidth="1"/>
+    <col min="11" max="11" width="14.375" style="10" customWidth="1"/>
+    <col min="12" max="12" width="14.625" style="10" customWidth="1"/>
+    <col min="13" max="13" width="30" style="10" customWidth="1"/>
+    <col min="14" max="14" width="104.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="11" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -658,117 +682,117 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="12"/>
+      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="16" t="s">
+      <c r="C3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="16" t="s">
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="13"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="13"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="13"/>
+      <c r="G4" s="12"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -851,27 +875,27 @@
       <c r="N1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -886,10 +910,10 @@
       <c r="J2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="16" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
@@ -898,25 +922,25 @@
       <c r="N2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="12"/>
+      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -931,15 +955,15 @@
       <c r="J3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="16" t="s">
         <v>24</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="15" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1032,95 +1056,95 @@
       <c r="N1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="3">
         <v>22419862</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="15" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="12"/>
+      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="3">
         <v>22419862</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="15" t="s">
         <v>24</v>
       </c>
       <c r="M3" s="3"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16" t="s">
+      <c r="N3" s="15"/>
+      <c r="O3" s="15" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1145,26 +1169,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="11.125" customWidth="1"/>
     <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="11" customWidth="1"/>
-    <col min="8" max="9" width="14.375" style="11" customWidth="1"/>
-    <col min="10" max="10" width="20.375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="10" customWidth="1"/>
+    <col min="8" max="9" width="14.375" style="10" customWidth="1"/>
+    <col min="10" max="10" width="20.375" style="10" customWidth="1"/>
     <col min="11" max="11" width="14.375" customWidth="1"/>
     <col min="12" max="12" width="14.625" customWidth="1"/>
     <col min="13" max="13" width="23.375" customWidth="1"/>
     <col min="14" max="14" width="27.625" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1207,42 +1232,45 @@
       <c r="N1" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="18" t="s">
+      <c r="O1" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="16" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
@@ -1251,29 +1279,59 @@
       <c r="N2" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" s="10" customFormat="1">
+      <c r="A3" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="13"/>
+      <c r="G4" s="12"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -1282,7 +1340,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1302,7 +1360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1310,9 +1368,9 @@
   <cols>
     <col min="1" max="1" width="11.125" customWidth="1"/>
     <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="11" customWidth="1"/>
-    <col min="8" max="9" width="14.375" style="11" customWidth="1"/>
-    <col min="10" max="10" width="20.375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="10" customWidth="1"/>
+    <col min="8" max="9" width="14.375" style="10" customWidth="1"/>
+    <col min="10" max="10" width="20.375" style="10" customWidth="1"/>
     <col min="11" max="11" width="14.375" customWidth="1"/>
     <col min="12" max="12" width="14.625" customWidth="1"/>
     <col min="13" max="13" width="10.375" customWidth="1"/>
@@ -1363,95 +1421,95 @@
       <c r="N1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="16" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="18" t="s">
+      <c r="N2" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="12"/>
+      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="16" t="s">
+      <c r="C3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="16" t="s">
         <v>24</v>
       </c>
       <c r="M3" s="3"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="16" t="s">
+      <c r="N3" s="17"/>
+      <c r="O3" s="15" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1462,7 +1520,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="13"/>
+      <c r="G4" s="12"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -1489,10 +1547,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1503,9 +1561,10 @@
     <col min="10" max="10" width="22.125" customWidth="1"/>
     <col min="11" max="11" width="14.375" customWidth="1"/>
     <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="13" max="13" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1539,29 +1598,32 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="18" t="s">
+      <c r="M1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="21"/>
+      <c r="O1" s="5"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1576,30 +1638,60 @@
       <c r="J2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="M2" s="11"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" s="10" customFormat="1">
+      <c r="A3" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="23"/>
+      <c r="O3" s="24"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1623,7 +1715,7 @@
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:J4</xm:sqref>
+          <xm:sqref>G2:J2 G4:J4 G3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>